<commit_message>
update of the code and results
</commit_message>
<xml_diff>
--- a/code/coronavirus_symptoms.xlsx
+++ b/code/coronavirus_symptoms.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agutf\Sync\school-flu\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D360D8B6-B002-49B3-AD6F-8BB8866EF9CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F642820-554D-4E48-9A2B-06964135CD01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="21378" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2778" yWindow="2778" windowWidth="15888" windowHeight="9444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="v2" sheetId="2" r:id="rId1"/>
-    <sheet name="coronavirus_symptoms_v1" sheetId="1" r:id="rId2"/>
+    <sheet name="final" sheetId="2" r:id="rId1"/>
+    <sheet name="analysis" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="39">
   <si>
     <t>Time</t>
   </si>
@@ -57,75 +57,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>R0 comparable to flu - total shedding should be comparable (13.6 day-logTiters)</t>
-  </si>
-  <si>
-    <t>Calculated days log-titers</t>
-  </si>
-  <si>
-    <t>Manore: an incubation period of 5.2</t>
-  </si>
-  <si>
-    <t>Holshoe: Fever for 10 days (1 human case in the US)</t>
-  </si>
-  <si>
-    <t>Chan - Patient 7after 4 days feel weakness, 4 more fever</t>
-  </si>
-  <si>
-    <t>Chan - 3-5 days to first symptom</t>
-  </si>
-  <si>
-    <t>Chan - 6-10 days to developing severe symptoms</t>
-  </si>
-  <si>
-    <t>Anderson:  in SARS virus is found naso-pharyngially on day 3 after first symptoms and peaks on 12</t>
-  </si>
-  <si>
-    <t>We show respiratory syndroms for the majority of cases who recover and not those that develop catastrophic ARS</t>
-  </si>
-  <si>
-    <t>Carrat: Systemic symptoms (fever, muscle aches, fatigue, headache)</t>
-  </si>
-  <si>
-    <t>Logically, some shedding occurs from day 1</t>
-  </si>
-  <si>
-    <t>We assume that viral shedding rises linearly in log scale until a peak on day 15 and then declines linearly by day 24</t>
-  </si>
-  <si>
-    <t>We assume severity of systemic symptoms lags the severity of respiratory symptoms by two days.</t>
-  </si>
-  <si>
-    <t>Bai - onset of symptoms in 3-14 of exposure (https://jamanetwork.com/journals/jama/fullarticle/2762028)</t>
-  </si>
-  <si>
-    <t>ReturnA</t>
-  </si>
-  <si>
-    <t>ReturnB</t>
-  </si>
-  <si>
-    <t>ReturnC</t>
-  </si>
-  <si>
-    <t>ReturnA = no policy rate and baseline parameters</t>
-  </si>
-  <si>
-    <t>ReturnB = ReturnA with 1 day policy rate and baseline compliance</t>
-  </si>
-  <si>
-    <t>ReturnC = ReturnA with 1 day policy rate and 100% compliance</t>
-  </si>
-  <si>
-    <t>New ILI cases start at day 3 and peak at 6 and 7 from infection (these are NEW cases, i.e., first occurance of fever)</t>
-  </si>
-  <si>
-    <t>Wu: 81% of the cases are clinically mild, unlike influenza where most naive cases are quite severe</t>
-  </si>
-  <si>
-    <t>He data for shedding</t>
-  </si>
-  <si>
     <t>The shedding rate appears to rise at this point in He et al. 2020</t>
   </si>
   <si>
@@ -138,7 +69,85 @@
     <t>Return C</t>
   </si>
   <si>
-    <t xml:space="preserve">Return rates: A = no policy rate and, B = 1 day policy rate with 0.5 compliance, C = 1 day policy rate and 100% compliance.  Rows are days from the time of infection. </t>
+    <t>Cheng H-Y, Jian S-W, Liu D-P, et al. High transmissibility of COVID-19 near symptom onset. Infectious Diseases (except HIV/AIDS). medRxiv; 2020.</t>
+  </si>
+  <si>
+    <t>He X, Lau EHY, Wu P, et al. Temporal dynamics in viral shedding and transmissibility of COVID-19. medRxiv. Cold Spring Harbor Laboratory Press; 2020; :2020.03.15.20036707.</t>
+  </si>
+  <si>
+    <t>Woelfel R, Corman VM, Guggemos W, et al. Clinical presentation and virological assessment of hospitalized cases of coronavirus disease 2019 in a travel-associated transmission cluster. medRxiv. Cold Spring Harbor Laboratory Press; 2020; :2020.03.05.20030502.</t>
+  </si>
+  <si>
+    <t>Fever</t>
+  </si>
+  <si>
+    <t>Sources for transmissibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wang Y, Jiang W, He Q, et al. Early, low-dose and short-term application of corticosteroid treatment in patients with severe COVID-19 pneumonia: single-center experience from Wuhan, China. Infectious Diseases (except HIV/AIDS). medRxiv; 2020.70.     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chan JF-W, Yuan S, Kok K-H, et al. A familial cluster of pneumonia associated with the 2019 novel coronavirus indicating person-to-person transmission: a study of a family cluster. Lancet. 2020; 395(10223):514–523.71.     </t>
+  </si>
+  <si>
+    <t>Holshue ML, DeBolt C, Lindquist S, et al. First Case of 2019 Novel Coronavirus in the United States. N Engl J Med. 2020; 382(10):929–936.</t>
+  </si>
+  <si>
+    <t>Cough</t>
+  </si>
+  <si>
+    <t>No data</t>
+  </si>
+  <si>
+    <t>Nasal</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Mostly absent</t>
+  </si>
+  <si>
+    <t>Rough guesses from Fever severity</t>
+  </si>
+  <si>
+    <t>The data was digitized and then linearly interpolated to day 5 and then after day 26</t>
+  </si>
+  <si>
+    <t>Simple segmented model based on case reportes</t>
+  </si>
+  <si>
+    <t>Separately, based on 77 transmission pairs obtained from publicly available sources within and outside mainland China, the serial interval was estimated to have a mean of 5.8 days (95% confidence interval [CI] = 4.8 to 6.8) and median of 5.2 days (95% CI = 4.1 to 6.4) based on a fitted gamma distribution (Figure 1b). Assuming an incubation period with a mean of 5.2 days from a separate study of early COVID-19 cases,2 we inferred that infectiousness started from 2.5 days before symptom onset and reached its peak at 0.6 days before symptom onset (Figure 1b). The proportion of transmission before symptom onset (area under the curve) was 44%. Infectiousness was estimated to decline relatively quickly within 7 days of illness onset</t>
+  </si>
+  <si>
+    <t>He et al:</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>incubation</t>
+  </si>
+  <si>
+    <t>first infectiousness</t>
+  </si>
+  <si>
+    <t>first symptom 5.2</t>
+  </si>
+  <si>
+    <t>peak infectiousness 4.6</t>
+  </si>
+  <si>
+    <t>peak infectiousness</t>
+  </si>
+  <si>
+    <t>first infectious 2.7</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Updated 9/8/2020 to data from Poletti et al.</t>
   </si>
 </sst>
 </file>
@@ -148,7 +157,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,27 +293,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -486,12 +481,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -657,17 +646,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -750,18 +737,10 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'v2'!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ViralShedding</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Infectiousness (relative)</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -770,8 +749,8 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -780,6 +759,7 @@
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -788,100 +768,100 @@
             <c:strLit>
               <c:ptCount val="32"/>
               <c:pt idx="0">
-                <c:v>1.000</c:v>
+                <c:v>1</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>2.000</c:v>
+                <c:v>2</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v>3.000</c:v>
+                <c:v>3</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>4.000</c:v>
+                <c:v>4</c:v>
               </c:pt>
               <c:pt idx="4">
-                <c:v>5.000</c:v>
+                <c:v>5</c:v>
               </c:pt>
               <c:pt idx="5">
-                <c:v>6.000</c:v>
+                <c:v>6</c:v>
               </c:pt>
               <c:pt idx="6">
-                <c:v>7.000</c:v>
+                <c:v>7</c:v>
               </c:pt>
               <c:pt idx="7">
-                <c:v>8.000</c:v>
+                <c:v>8</c:v>
               </c:pt>
               <c:pt idx="8">
-                <c:v>9.000</c:v>
+                <c:v>9</c:v>
               </c:pt>
               <c:pt idx="9">
-                <c:v>10.000</c:v>
+                <c:v>10</c:v>
               </c:pt>
               <c:pt idx="10">
-                <c:v>11.000</c:v>
+                <c:v>11</c:v>
               </c:pt>
               <c:pt idx="11">
-                <c:v>12.000</c:v>
+                <c:v>12</c:v>
               </c:pt>
               <c:pt idx="12">
-                <c:v>13.000</c:v>
+                <c:v>13</c:v>
               </c:pt>
               <c:pt idx="13">
-                <c:v>14.000</c:v>
+                <c:v>14</c:v>
               </c:pt>
               <c:pt idx="14">
-                <c:v>15.000</c:v>
+                <c:v>15</c:v>
               </c:pt>
               <c:pt idx="15">
-                <c:v>16.000</c:v>
+                <c:v>16</c:v>
               </c:pt>
               <c:pt idx="16">
-                <c:v>17.000</c:v>
+                <c:v>17</c:v>
               </c:pt>
               <c:pt idx="17">
-                <c:v>18.000</c:v>
+                <c:v>18</c:v>
               </c:pt>
               <c:pt idx="18">
-                <c:v>19.000</c:v>
+                <c:v>19</c:v>
               </c:pt>
               <c:pt idx="19">
-                <c:v>20.000</c:v>
+                <c:v>20</c:v>
               </c:pt>
               <c:pt idx="20">
-                <c:v>21.000</c:v>
+                <c:v>21</c:v>
               </c:pt>
               <c:pt idx="21">
-                <c:v>22.000</c:v>
+                <c:v>22</c:v>
               </c:pt>
               <c:pt idx="22">
-                <c:v>23.000</c:v>
+                <c:v>23</c:v>
               </c:pt>
               <c:pt idx="23">
-                <c:v>24.000</c:v>
+                <c:v>24</c:v>
               </c:pt>
               <c:pt idx="24">
-                <c:v>25.000</c:v>
+                <c:v>25</c:v>
               </c:pt>
               <c:pt idx="25">
-                <c:v>26.000</c:v>
+                <c:v>26</c:v>
               </c:pt>
               <c:pt idx="26">
-                <c:v>27.000</c:v>
+                <c:v>27</c:v>
               </c:pt>
               <c:pt idx="27">
-                <c:v>28.000</c:v>
+                <c:v>28</c:v>
               </c:pt>
               <c:pt idx="28">
-                <c:v>29.000</c:v>
+                <c:v>29</c:v>
               </c:pt>
               <c:pt idx="29">
-                <c:v>30.000</c:v>
+                <c:v>30</c:v>
               </c:pt>
               <c:pt idx="30">
-                <c:v>31.000</c:v>
+                <c:v>31</c:v>
               </c:pt>
               <c:pt idx="31">
-                <c:v>32.000</c:v>
+                <c:v>32</c:v>
               </c:pt>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -895,11 +875,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'v2'!$B$2:$B$34</c15:sqref>
+                    <c15:sqref>final!$B$2:$B$34</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'v2'!$B$2:$B$33</c:f>
+              <c:f>final!$B$2:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="32"/>
@@ -1013,29 +993,20 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'v2'!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>SystemicSymptoms</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Fever</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
@@ -1044,6 +1015,7 @@
                 <a:solidFill>
                   <a:schemeClr val="accent2"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1159,11 +1131,11 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'v2'!$C$2:$C$34</c15:sqref>
+                    <c15:sqref>final!$C$2:$C$34</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'v2'!$C$2:$C$33</c:f>
+              <c:f>final!$C$2:$C$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -1293,6 +1265,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1300,7 +1286,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1313,7 +1299,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:rPr lang="en-US"/>
                   <a:t>Day from infection</a:t>
                 </a:r>
               </a:p>
@@ -1332,7 +1318,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1370,7 +1356,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1401,28 +1387,33 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
+        <c:minorGridlines>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln>
               <a:solidFill>
                 <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+        </c:minorGridlines>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1459,7 +1450,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1502,7 +1493,7 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="lt1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -1574,7 +1565,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1585,7 +1576,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -1608,18 +1599,18 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="bg1"/>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -1631,7 +1622,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -1639,11 +1630,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -1675,35 +1666,45 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="22225" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1715,30 +1716,34 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1760,15 +1765,13 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1783,15 +1786,15 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1802,17 +1805,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -1821,10 +1823,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
@@ -1840,21 +1842,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1873,17 +1869,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -1892,17 +1887,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -1911,17 +1905,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -1942,7 +1935,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -1950,7 +1943,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -1963,6 +1956,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1970,10 +1974,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -1994,7 +1998,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2003,14 +2007,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2024,7 +2028,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
@@ -2040,8 +2044,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2057,6 +2061,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2064,14 +2079,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2081,15 +2090,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>49530</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>78104</xdr:rowOff>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>1905</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>179069</xdr:rowOff>
+      <xdr:colOff>424815</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>60959</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2414,10 +2423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ABAE5D2-E623-4190-AAB1-F2C79B0651E2}">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2448,36 +2457,37 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="J1" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="L1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="2">
         <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
       </c>
       <c r="F2">
         <f>SUM(C2:E2)</f>
@@ -2495,25 +2505,25 @@
       <c r="J2">
         <v>1</v>
       </c>
-      <c r="K2" t="s">
-        <v>30</v>
+      <c r="L2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="2">
         <v>0.25</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F33" si="0">SUM(C3:E3)</f>
@@ -2530,24 +2540,27 @@
       </c>
       <c r="J3">
         <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="2">
         <v>0.5</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="1">
         <f>C$8*(A4-2)/5</f>
         <v>0.17599999999999999</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
@@ -2565,23 +2578,26 @@
       <c r="J4">
         <v>1</v>
       </c>
+      <c r="M4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="2">
         <v>0.75</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="1">
         <f t="shared" ref="C5:C7" si="1">C$8*(A5-2)/5</f>
         <v>0.35199999999999998</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
@@ -2591,31 +2607,34 @@
         <v>0.1</v>
       </c>
       <c r="H5">
-        <v>0.87</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="I5">
-        <v>0.86</v>
+        <v>0.97099999999999997</v>
       </c>
       <c r="J5">
-        <v>0.85</v>
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="M5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4">
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
         <f t="shared" si="1"/>
         <v>0.52800000000000002</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
@@ -2625,31 +2644,34 @@
         <v>0.15</v>
       </c>
       <c r="H6">
-        <v>0.74</v>
+        <v>0.94699999999999995</v>
       </c>
       <c r="I6">
-        <v>0.72</v>
+        <v>0.94199999999999995</v>
       </c>
       <c r="J6">
-        <v>0.69</v>
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="2">
         <v>0.84514066408418953</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="1">
         <f t="shared" si="1"/>
         <v>0.70399999999999996</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
@@ -2659,30 +2681,33 @@
         <v>0.2</v>
       </c>
       <c r="H7">
-        <v>0.61</v>
+        <v>0.92</v>
       </c>
       <c r="I7">
-        <v>0.56999999999999995</v>
+        <v>0.91200000000000003</v>
       </c>
       <c r="J7">
-        <v>0.54</v>
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="L7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="2">
         <v>0.72111438658953153</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="1">
         <v>0.88</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
@@ -2692,30 +2717,33 @@
         <v>0.2</v>
       </c>
       <c r="H8">
-        <v>0.48</v>
+        <v>0.89400000000000002</v>
       </c>
       <c r="I8">
-        <v>0.43</v>
+        <v>0.88300000000000001</v>
       </c>
       <c r="J8">
-        <v>0.38</v>
+        <v>0.873</v>
+      </c>
+      <c r="L8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="2">
         <v>0.61114087465065914</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="1">
         <v>0.86</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
@@ -2725,30 +2753,33 @@
         <v>0.15</v>
       </c>
       <c r="H9">
-        <v>0.36</v>
+        <v>0.86699999999999999</v>
       </c>
       <c r="I9">
-        <v>0.28999999999999998</v>
+        <v>0.85399999999999998</v>
       </c>
       <c r="J9">
-        <v>0.23</v>
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="L9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="2">
         <v>0.5398813858918956</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="1">
         <v>0.84</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
@@ -2758,30 +2789,33 @@
         <v>0.1</v>
       </c>
       <c r="H10">
-        <v>0.37</v>
+        <v>0.871</v>
       </c>
       <c r="I10">
-        <v>0.31</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="J10">
-        <v>0.24</v>
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="L10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="2">
         <v>0.47309102035858192</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="1">
         <v>0.82</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
@@ -2791,30 +2825,30 @@
         <v>0.05</v>
       </c>
       <c r="H11">
-        <v>0.39</v>
+        <v>0.874</v>
       </c>
       <c r="I11">
-        <v>0.32</v>
+        <v>0.86099999999999999</v>
       </c>
       <c r="J11">
-        <v>0.26</v>
+        <v>0.84799999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="2">
         <v>0.42652522117788311</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="1">
         <v>0.8</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
@@ -2824,30 +2858,33 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>0.4</v>
+        <v>0.877</v>
       </c>
       <c r="I12">
-        <v>0.34</v>
+        <v>0.86399999999999999</v>
       </c>
       <c r="J12">
-        <v>0.28000000000000003</v>
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="2">
         <v>0.40013858361456112</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="1">
         <v>0.78</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
@@ -2857,30 +2894,33 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>0.41</v>
+        <v>0.88</v>
       </c>
       <c r="I13">
-        <v>0.36</v>
+        <v>0.86699999999999999</v>
       </c>
       <c r="J13">
-        <v>0.3</v>
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="L13" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="2">
         <v>0.37933672848536482</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="1">
         <v>0.76</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>37</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
@@ -2890,30 +2930,30 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <v>0.43</v>
+        <v>0.88300000000000001</v>
       </c>
       <c r="I14">
-        <v>0.37</v>
+        <v>0.871</v>
       </c>
       <c r="J14">
-        <v>0.31</v>
+        <v>0.85899999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="2">
         <v>0.3512928180859004</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="1">
         <v>0.66</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
@@ -2923,30 +2963,33 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <v>0.44</v>
+        <v>0.88600000000000001</v>
       </c>
       <c r="I15">
-        <v>0.39</v>
+        <v>0.874</v>
       </c>
       <c r="J15">
-        <v>0.33</v>
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="2">
         <v>0.31762628797294812</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
@@ -2956,30 +2999,33 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>0.52</v>
+        <v>0.90100000000000002</v>
       </c>
       <c r="I16">
-        <v>0.47</v>
+        <v>0.89100000000000001</v>
       </c>
       <c r="J16">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="L16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="2">
         <v>0.28675431120730649</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="1">
         <v>0.44</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>37</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
@@ -2989,30 +3035,30 @@
         <v>0</v>
       </c>
       <c r="H17">
-        <v>0.6</v>
+        <v>0.91700000000000004</v>
       </c>
       <c r="I17">
-        <v>0.56000000000000005</v>
+        <v>0.90900000000000003</v>
       </c>
       <c r="J17">
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>0.90100000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="2">
         <v>0.24409872458259479</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="1">
         <v>0.33</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
+        <v>37</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
@@ -3022,30 +3068,33 @@
         <v>0</v>
       </c>
       <c r="H18">
-        <v>0.68</v>
+        <v>0.93400000000000005</v>
       </c>
       <c r="I18">
-        <v>0.65</v>
+        <v>0.92700000000000005</v>
       </c>
       <c r="J18">
-        <v>0.61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>0.92</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="2">
         <v>0.20651009019728281</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="1">
         <v>0.22</v>
       </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" t="s">
+        <v>37</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
@@ -3055,30 +3104,33 @@
         <v>0</v>
       </c>
       <c r="H19">
-        <v>0.76</v>
+        <v>0.95</v>
       </c>
       <c r="I19">
-        <v>0.73</v>
+        <v>0.94499999999999995</v>
       </c>
       <c r="J19">
-        <v>0.71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>0.94</v>
+      </c>
+      <c r="L19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="2">
         <v>0.17675052944494302</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="1">
         <v>0.11</v>
       </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="s">
+        <v>37</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
@@ -3088,30 +3140,30 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <v>0.84</v>
+        <v>0.96699999999999997</v>
       </c>
       <c r="I20">
-        <v>0.82</v>
+        <v>0.96399999999999997</v>
       </c>
       <c r="J20">
-        <v>0.81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="2">
         <v>0.13858784947842331</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" t="s">
+        <v>37</v>
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
@@ -3121,33 +3173,33 @@
         <v>0</v>
       </c>
       <c r="H21">
-        <v>0.92</v>
+        <v>0.98299999999999998</v>
       </c>
       <c r="I21">
-        <v>0.91</v>
+        <v>0.98199999999999998</v>
       </c>
       <c r="J21">
-        <v>0.9</v>
+        <v>0.98</v>
       </c>
       <c r="K21" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="2">
         <v>0.11222067108734624</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" t="s">
+        <v>37</v>
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
@@ -3165,22 +3217,25 @@
       <c r="J22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L22" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="2">
         <v>9.4817684710161235E-2</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" t="s">
+        <v>37</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
@@ -3198,22 +3253,25 @@
       <c r="J23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="2">
         <v>8.1799498478699523E-2</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
+      <c r="D24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" t="s">
+        <v>37</v>
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
@@ -3232,21 +3290,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="2">
         <v>7.6843895947141666E-2</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" t="s">
+        <v>37</v>
       </c>
       <c r="F25">
         <f t="shared" si="0"/>
@@ -3265,21 +3323,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="2">
         <v>6.9527247183270691E-2</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
+      <c r="D26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" t="s">
+        <v>37</v>
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
@@ -3298,21 +3356,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="2">
         <v>6.6715396793963835E-2</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
+      <c r="D27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" t="s">
+        <v>37</v>
       </c>
       <c r="F27">
         <f t="shared" si="0"/>
@@ -3331,21 +3389,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="2">
         <v>5.5596163994969854E-2</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
+      <c r="D28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" t="s">
+        <v>37</v>
       </c>
       <c r="F28">
         <f t="shared" si="0"/>
@@ -3364,21 +3422,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="2">
         <v>4.4476931195975886E-2</v>
       </c>
       <c r="C29">
         <v>0</v>
       </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
+      <c r="D29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" t="s">
+        <v>37</v>
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
@@ -3397,21 +3455,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="2">
         <v>3.3357698396981918E-2</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
+      <c r="D30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" t="s">
+        <v>37</v>
       </c>
       <c r="F30">
         <f t="shared" si="0"/>
@@ -3430,21 +3488,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="2">
         <v>2.2238465597987943E-2</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
+      <c r="D31" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" t="s">
+        <v>37</v>
       </c>
       <c r="F31">
         <f t="shared" si="0"/>
@@ -3463,21 +3521,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="2">
         <v>1.1119232798993966E-2</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
+      <c r="D32" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" t="s">
+        <v>37</v>
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
@@ -3494,23 +3552,26 @@
       </c>
       <c r="J32">
         <v>1</v>
+      </c>
+      <c r="L32" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="2">
         <v>0</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
+      <c r="D33" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" t="s">
+        <v>37</v>
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
@@ -3528,9 +3589,6 @@
       <c r="J33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B34" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3540,880 +3598,134 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{365C6ED4-3F3E-48FC-AB7B-9586F7D34DCD}">
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="66" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="20.83984375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="144" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" t="s">
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2" s="3">
-        <v>1</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1</v>
-      </c>
-      <c r="J2" s="3">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0.09</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
-      <c r="I3" s="2">
-        <v>1</v>
-      </c>
-      <c r="J3" s="2">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3">
-        <v>13.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0.17</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2">
-        <v>1</v>
-      </c>
-      <c r="J4" s="2">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0.95599999999999996</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0.93400000000000005</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0.91200000000000003</v>
-      </c>
-      <c r="K5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.34</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0.91200000000000003</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0.86799999999999999</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0.82399999999999995</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0.43</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0.82399999999999995</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0.73599999999999999</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0.64800000000000002</v>
-      </c>
-      <c r="K7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0.51</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1.4</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="H8" s="2">
-        <v>0.78</v>
-      </c>
-      <c r="I8" s="2">
-        <v>0.67</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="K8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="H9" s="2">
-        <v>0.73599999999999999</v>
-      </c>
-      <c r="I9" s="2">
-        <v>0.60399999999999998</v>
-      </c>
-      <c r="J9" s="2">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="K9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0.69</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0.69199999999999995</v>
-      </c>
-      <c r="I10" s="2">
-        <v>0.53800000000000003</v>
-      </c>
-      <c r="J10" s="2">
-        <v>0.38400000000000001</v>
-      </c>
-      <c r="K10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0.77</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0.64800000000000002</v>
-      </c>
-      <c r="I11" s="2">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="J11" s="2">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="K11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0.86</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0.64800000000000002</v>
-      </c>
-      <c r="I12" s="2">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="K12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1">
-        <v>0.94</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0</v>
-      </c>
-      <c r="F13" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0.64800000000000002</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="K13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1">
-        <v>1.03</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
-      <c r="F14" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0</v>
-      </c>
-      <c r="H14" s="2">
-        <v>0.64800000000000002</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="J14" s="2">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="K14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2">
-        <v>0.64800000000000002</v>
-      </c>
-      <c r="I15" s="2">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="J15" s="2">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="K15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0</v>
-      </c>
-      <c r="H16" s="2">
-        <v>0.64800000000000002</v>
-      </c>
-      <c r="I16" s="2">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="J16" s="2">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="K16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1">
-        <v>1.07</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0</v>
-      </c>
-      <c r="F17" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0</v>
-      </c>
-      <c r="H17" s="2">
-        <v>0.64800000000000002</v>
-      </c>
-      <c r="I17" s="2">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="J17" s="2">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="K17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0.93</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0</v>
-      </c>
-      <c r="F18" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="G18" s="1">
-        <v>0</v>
-      </c>
-      <c r="H18" s="2">
-        <v>0.64800000000000002</v>
-      </c>
-      <c r="I18" s="2">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="J18" s="2">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="K18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="C19" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-      <c r="F19" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="G19" s="1">
-        <v>0</v>
-      </c>
-      <c r="H19" s="2">
-        <v>0.64800000000000002</v>
-      </c>
-      <c r="I19" s="2">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="J19" s="2">
-        <v>0.29599999999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1">
-        <v>0.67</v>
-      </c>
-      <c r="C20" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="D20" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0</v>
-      </c>
-      <c r="F20" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="G20" s="1">
-        <v>0</v>
-      </c>
-      <c r="H20" s="2">
-        <v>0.64800000000000002</v>
-      </c>
-      <c r="I20" s="2">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="J20" s="2">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="K20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="C21" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="D21" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="E21" s="1">
-        <v>0</v>
-      </c>
-      <c r="F21" s="1">
-        <v>1.4</v>
-      </c>
-      <c r="G21" s="1">
-        <v>0</v>
-      </c>
-      <c r="H21" s="2">
-        <v>0.64800000000000002</v>
-      </c>
-      <c r="I21" s="2">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="J21" s="2">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="K21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="C22" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="D22" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0</v>
-      </c>
-      <c r="F22" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="G22" s="1">
-        <v>0</v>
-      </c>
-      <c r="H22" s="2">
-        <v>0.64800000000000002</v>
-      </c>
-      <c r="I22" s="2">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="J22" s="2">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="K22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1">
-        <v>0.27</v>
-      </c>
-      <c r="C23" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="D23" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0</v>
-      </c>
-      <c r="F23" s="1">
-        <v>1</v>
-      </c>
-      <c r="G23" s="1">
-        <v>0</v>
-      </c>
-      <c r="H23" s="2">
-        <v>0.69199999999999995</v>
-      </c>
-      <c r="I23" s="2">
-        <v>0.53800000000000003</v>
-      </c>
-      <c r="J23" s="2">
-        <v>0.38400000000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1">
-        <v>0.13</v>
-      </c>
-      <c r="C24" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="D24" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="E24" s="1">
-        <v>0</v>
-      </c>
-      <c r="F24" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="G24" s="1">
-        <v>0</v>
-      </c>
-      <c r="H24" s="2">
-        <v>0.73599999999999999</v>
-      </c>
-      <c r="I24" s="2">
-        <v>0.60399999999999998</v>
-      </c>
-      <c r="J24" s="2">
-        <v>0.47199999999999998</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1">
-        <v>0</v>
-      </c>
-      <c r="C25" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="D25" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="E25" s="1">
-        <v>0</v>
-      </c>
-      <c r="F25" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="G25" s="1">
-        <v>0</v>
-      </c>
-      <c r="H25" s="2">
-        <v>0.78</v>
-      </c>
-      <c r="I25" s="2">
-        <v>0.67</v>
-      </c>
-      <c r="J25" s="2">
-        <v>0.56000000000000005</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>